<commit_message>
finished adding image urls
</commit_message>
<xml_diff>
--- a/CompleteNASDAQDataset.xlsx
+++ b/CompleteNASDAQDataset.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="223">
   <si>
     <t>Activision Blizzard</t>
   </si>
@@ -188,9 +188,6 @@
     <t>Mondelez</t>
   </si>
   <si>
-    <t>Monster Beverage</t>
-  </si>
-  <si>
     <t>Netease</t>
   </si>
   <si>
@@ -510,6 +507,195 @@
   </si>
   <si>
     <t>https://i0.wp.com/www.broadbandtvnews.com/wp-content/uploads/2015/05/Broadcom.logo_.png?resize=1200%2C597</t>
+  </si>
+  <si>
+    <t>https://mms.businesswire.com/media/20200526005569/en/633339/23/Cadence_Logo_2_Reg_Black.jpg</t>
+  </si>
+  <si>
+    <t>https://www.cerner.com/nl/-/media/code-media-folder/apps/cardiac-risk/cardiac-risk-logo-header.png?vs=1&amp;h=702&amp;w=1250&amp;la=en&amp;hash=0758D3526ABFE809F699C25D568272FAFE2CAAAD</t>
+  </si>
+  <si>
+    <t>https://pmcdeadline2.files.wordpress.com/2020/04/charter-communications-logo.jpg?w=1000</t>
+  </si>
+  <si>
+    <t>https://www.checkpoint.com/wp-content/uploads/CP_ltd_vertical_Pos.gif</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/8/8e/Cintas_logo.svg/1280px-Cintas_logo.svg.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/0/08/Cisco_logo_blue_2016.svg/1200px-Cisco_logo_blue_2016.svg.png</t>
+  </si>
+  <si>
+    <t>https://www.gala-global.org/sites/default/files/company_logo/Citrix_DirectoryLogo.gif</t>
+  </si>
+  <si>
+    <t>https://media-exp1.licdn.com/dms/image/C4E1BAQEn2A1bmxY6xA/company-background_10000/0?e=2159024400&amp;v=beta&amp;t=hwfkiJKy9nPasCiSKkgPtLKA1QlCSaNLUnksPLNrnPE</t>
+  </si>
+  <si>
+    <t>https://mms.businesswire.com/media/20200127005037/en/351493/23/Comcast-Logo.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/5/59/Costco_Wholesale_logo_2010-10-26.svg/1200px-Costco_Wholesale_logo_2010-10-26.svg.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/f/fe/CSX_transp_logo.svg</t>
+  </si>
+  <si>
+    <t>https://www.ishn.com/ext/resources/logos/logos2/dollar-tree-logo-422.png?t=1413550792&amp;width=696</t>
+  </si>
+  <si>
+    <t>https://www.ageuk.org.uk/bp-assets/globalassets/solihull/icons/ebay-logo.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/0/0d/Electronic-Arts-Logo.svg/1200px-Electronic-Arts-Logo.svg.png</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/kkf2Siy556vDQE_iqF0rAfmtdnHSo75AjBpRIfvCIxMruZdfGeb24S1UFDvb4wTQESg</t>
+  </si>
+  <si>
+    <t>https://cdn3.iconfinder.com/data/icons/facebook-ui-flat/48/Facebook_UI-03-512.png</t>
+  </si>
+  <si>
+    <t>https://www.fastenal.com/static/images/logos/fastenal/fastenal-logo-darkblue-white.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/8/89/Fiserv_logo.svg/1200px-Fiserv_logo.svg.png</t>
+  </si>
+  <si>
+    <t>https://dev.rodpub.com/images/192/303_main.jpg</t>
+  </si>
+  <si>
+    <t>https://download.logo.wine/logo/Idexx_Laboratories/Idexx_Laboratories-Logo.wine.png</t>
+  </si>
+  <si>
+    <t>https://assets.illumina.com/content/dam/illumina-common/logo/illumina-full_logo-RGB-black.svg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/en/thumb/5/5a/Incyte_logo.svg/1200px-Incyte_logo.svg.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/c/c9/Intel-logo.svg/1200px-Intel-logo.svg.png</t>
+  </si>
+  <si>
+    <t>https://logos-download.com/wp-content/uploads/2016/05/Intuit_logo_logotype.png</t>
+  </si>
+  <si>
+    <t>https://ortoday.com/wp-content/uploads/2019/07/HEADER-NAV_LOGO_IMG-en-us-1533756092686.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/en/c/c4/JD.com_logo.png</t>
+  </si>
+  <si>
+    <t>https://photos.prnewswire.com/prnfull/20140123/SF50413LOGO</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/en/thumb/a/ac/Lam_Research_logo.svg/1200px-Lam_Research_logo.svg.png</t>
+  </si>
+  <si>
+    <t>https://halberdbastion.com/sites/default/files/2017-07/Liberty-Global-Logo.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/b/b3/Marriott_hotels_logo14.svg/1200px-Marriott_hotels_logo14.svg.png</t>
+  </si>
+  <si>
+    <t>https://photos.prnewswire.com/prnfull/20120912/SF71654LOGO</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/en/thumb/2/20/MercadoLibre.svg/1200px-MercadoLibre.svg.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/c/ca/Microchip-Logo.svg/1200px-Microchip-Logo.svg.png</t>
+  </si>
+  <si>
+    <t>https://www.exportnow.com/wp-content/uploads/2017/10/logo-micron.png</t>
+  </si>
+  <si>
+    <t>https://www.mustardit.co.uk/wp-content/uploads/2019/01/01-750x300.png</t>
+  </si>
+  <si>
+    <t>https://www.mondelezinternational.com/-/media/Mondelez/Media/Asset-Library/logos/MDLZlogo.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/en/8/89/Monster_Energy_logo.png</t>
+  </si>
+  <si>
+    <t>Monster Beverages</t>
+  </si>
+  <si>
+    <t>https://netease-na.com/wp-content/uploads/2016/11/netease-logo-big.png</t>
+  </si>
+  <si>
+    <t>https://parentzone.org.uk/sites/default/files/580b57fcd9996e24bc43c529.png</t>
+  </si>
+  <si>
+    <t>https://static1.purestorage.com/content/dam/purestorage/pure-events/nvidia.png.imgo.png</t>
+  </si>
+  <si>
+    <t>https://vignette.wikia.nocookie.net/logopedia/images/c/c3/OReillyAutopartsLogo.jpg/revision/latest?cb=20150921175728</t>
+  </si>
+  <si>
+    <t>https://logos-download.com/wp-content/uploads/2016/11/PACCAR_logo_blue.png</t>
+  </si>
+  <si>
+    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAgcAAABhCAMAAAB1TfJnAAAAt1BMVEX///8AS40ARYoAR4tTga8ASYwAQ4kAQYgAPocAQIgANINJealyl7xYg68APIYAOoV/nL3K2ecMUJGYqcTz9/pWe6gAN4SwxNjy9vnd5u/r8vezv9Pk6/IbW5eiudGZsszU3+oAVJQ0aqBHc6RkjbaEpMRigKpxjbOPq8eetM28yttpkLgfYZtMc6QYWZZ9n8EpZ59DbaG7x9kAG3p6lLeRpcJsibGpuM9BaZ01b6O4zd+duNHM3OnMVhQgAAAU8UlEQVR4nO1dbVebzBYljDNAo4lJ0bw0JkRNjfGl2mu1Wv//77qBAQJkbxjgWbfrWTf7S9cqZhhmzpz3c8ayDjjggAMOOOCAAw444IADDjjggAMOOADDn/7tGfwNTCfBaL36cXx3vFrMfw6Cyf/lKqQY376ffX//Mfvb8/jfYrZ4ebhQruc4ylbK89yeuri6WQ/+9rz+Hrqr7TmY3l5OKv/y+sgEJ9vj9W0QmB2uyQkcozsKH3508UO6WT6fYfd492fTzZ04d2xbyk4GUgrl9N27zbhswnd4+Gv4xyP8AUefpU/N0H1kD+ZwLlMy8xB3Y8vfLvnqdDGwBheVO3duG2F7vFzv8fllVDVeuKwuHKJ3Gj6c9BV8+IONtvDonIYp8QSnz0rlKCAHpR4WPp3vtAOH97p1vq6jj9wLfmoIIcgD5xkS8jVfG3u7NoMna3K/2Vy9WTfrij0b9Oji7WN7uHrD0yoeE3zBv7a/h0/9Ixs9FM9sNI/OppcQ5aZ77ghOBdHMXXHLeMKHhL/1btEf+/fwj+V99HR6JcqmUQXRhYuzRQ/xy/k5G0jKcG3u3qzJw/b7vlubq4pNW9BlZm9wHhelI/rfybeI54g53So47CPWZXy6Mh11qv8kOOnQv8m+QV0S2UNmJDboj6f44Ngn0dPJYyk5VsGZ41OyHR8IqcGQvsyJaLi72U5ovb68tSbPFYLhBq5BKYR79Vky4ohRlnyMOMkEzp6surV22DRUN+L0/rpnQgXRxNUpFA4vhDID9McfLhzb0YdjgJ8aQqrJgGytHO5t5HRJeY+nj8jRT2tyMRdb3eLzmYvFaKyHJnzMfsSbFoHOTiq9sFdw39QvNNjEZiQvNAOZXdYhZO8MCLXxO5yx+A0/7wcmzJ7+Nk62JhD3M+uMMYSipui/0i93Y065fgnlwtuWVb2d8A0LETTjY9KhhFCyEj39ozk8M/YVoFi/y75ViojJz5f1+JkCh3yKl8DGS3cGiUYutVjrtlMPznxr0MfP7JPC+qyoRPfO4j+Zydnsybe2euJTycENsamrHsSQSyJrg2WJ1r7Ss8NiTQE1bkHJQPPhlVOXjMU+IZCVd6AaNH2Cbwx3MESnlXoQaTxEIZJenpWNuN50loqQ0WX4tbM/16flZNCcj4kLPOBJyYDxCSMMrbdPsjMqFZyTaKAGs7efinyHrMF5gL5vMMTz0Qs9KbdaquCFvH9ExvBWuaW5YJxHLDOaxNv9r9HH7dWqXDuwrHdTHWt/WpDENnTnOqltZc0hHajj4mA+k5UdO1R7pmeNmJnzvbAoWEWXQ2hmfsNEo7T0HtXXurNwg3AQrD9tVy8zb5+qReK+wDd+/PhT6kSL0HzecglUrhIrL/qN/qsp1sseiqPNGVHJTiiVvjeUaV5B48KcHuorlnUK6SDWVqxfrdRE2Y8G2RANoZNhmCsqMKGjoQoT6oiohg1cE3P2CXqOdkw6UJvas9OmbHLS24TMoiEZbDctR8FEo3Gg/WJdYjVxGD2krhMziEs9CmGDzks6ixFdmk6FQogxamPu9vY8P1MqtDTsj5LXSrvwCdS14YULctqUDLbTyIk0Io/VG1wxD6uJegdn2NdoikQyjjAflJ2Ev3Nl3MVxiCpgLmcIZ1V3OBV7amcX6DtUXuOYs41WR37oA2yx5HaWIXzFkx5C/spsCx0dmWAqMYWbHATMdNJNHt8TtiNVVRgBox0fE1cFF9ekynhOeS086uIpO9h0SEaLPGtBK8U8p5KeYDXxAqoHxA0f72Ar9rpFEL+FjCNiv8ANOyHOXSMyaMvH7CA/HF7R7A9e48XFvufzrF57TaRCJAHHz+0EcSYM60PeBLWfLYgPT2oGc9dqVvIyEbQ+jlbJZeTPXzNW6FQ4DSmCMiuvGoWA3KbyjIo02gHpwM0EtUfMQ+QuoqUof49yPE/xTZH27k0zzOkVjIOPsRteXOrvemrlTdTxWP31+Pucr9tnAyovK2IIHC35WMHzel+5CrugIrTZ1U4hnjJ/d0Tzk5J5S7unuqdf325/nUgagVInVWsAvFoWdcOrGz1pHv8zgZPRjzCTko8hDyfLbF82zj67bsXHCj7FtQFRuYmCBv3Z4iElaBwCDNl1ePJKBJCQZx/JKP7HGfXzpm86JpweLuqGnFOtnpE8BlPk2CE+9P2B9U5WRpDAvQmIeuB9SdH3yhI8ZIYRcUdnBukpmyCq3nkQNkQqSCf8iwF9k3Qufua+cERkaT+1BrCxnnD6AtZ4exxtD78Rkup/McJ/Mhs5fYbfaB/fktMmOh+NyWCMj5WXsZyD+emDoMuedcjcmZigO1MTHng33kTqh5ARHT1RdmDvKcwD/Iep+CdsNiOisiAuX3fMv2lreTQ5qERcSbYXXnMysAbEX5EXjePBI1Pdxc7GDnomPFGlWTUfKK0nsedOyQvd6DmLzG6f73k0mAc21clI3EjhnCvi+dfexDHW8kkeQxVqGcbSa+Y40FjAI1wMVGzxQs76Tu3mIaH8fHcuAvT3chk92hCvqTrTr2LMQsDFgMqbSHTrb5DTSwGPF3HDx/oyDpuA+JkRqBsNoVeeKliBF7h39l68x/KJH1OldEBcoUWECm8M6B84D6XylLjTYk0ooLFo7EW5gz6rhNiZCxSqB4RZx/YzSflt6OplqwC//KbRK5I3YV0E0S/xvarUgUDlVgHDIPkFjFBHa0a2RkothZgiIh73ph0Bbo9M3MYkbnQPh8LyKsm3W5GMtYZ6/B9jo95r6EaMMcOi0fuz/6fERZTSAdSjwU+kTPnt9Dd4HqpnA+Kkj/ODfGYKkkRXa4I+UyZKENZE9vXNCFgiiQvNW0hC/kV19B/D1BthXzV9gwbRt85BXsEAC4Y4+8KaoMcC/afaMUlkuIuH6RhzqY4Tq5g4iWU7MjsUM5hfoLRpEjBv4udgHyNsZ8c5aT62PPbyCo1xa6Yh2PctqxcxH5NDMO/BEk8h1g9OwN7YXeSlykT1ERnK5YRkWKRBLazUdKTLymuml67ax5dv0UOsKm8XAYJoSdoP+EnyGL423Z/ZpQlDiKsBWgDn1gpUzbWBnjJpayE7AF4faW/QGqvX3aCQX6yw4yfN0iR5ohmLtAh/cQrwoqd+wyK4+L8h4vwmrCpL2SgxJIKJh1aI1lW82FcO83BIKqeMzii0m+0rawM+Q1zuZBnUB5lNmFgmtFCk0XL7jco3CogFKctJOzk2AGTtzEzLoGH+URYB8aB8A3+L/XuxuQ8t3f4Gyl6ZSabdmB86N43+EaVcNIu1TXA8pxakq8eiFWlAKhXgLHHVWXU2eQ8o9TWBE+BhYQJhULrmDpZXha6VGVrj/o7y/d+mh1HtkgGIZ9dp5k8rTa82hHjXX9Mi2EiSHaxpRX6IVMCBWhfYJyDu90lzTj6xF7GOX0Cxk2EmIsw+y8ZzSagPzGmnCpF4NDJyDPDWPMkxRawmkjwGsyGYy5HXLEVw2zkOIhD3bJL7tMPk+JwE/yJNFdal26GyCfWG7MElRtvee5wdi/rEf8KqaqpQmUFlgLjEr5YfuACc7BAuYamGoI6afXUOUywaC8mn09ELS4qMdX+0lHrn/FfwKFu/7RPdvzBYNvmS+K9RVbgJqhWx6unpZDFj5oaGUNQDUFYQoYr5oY0wIR6Ul28x3lZ3V8Nz16ZCvBf6BmHWd2wdIoMg1+/CqOzDyzLNW/wLByeZV2Hconxj90F6N1pYHvKJbig5rdGL+a/qgPEx5cbwlF2qRUUxI/8SsQNbHxHkQBDZ6iwS9M3BzmWEkHKihkY66WVQC3EEGybWGEKVhIl4fxXbpEVRNdrl1m7hhfNYwDSCOPsPuYDzVUvVHjMxzGqAUNTQlhWVIEZoLcSCdNNmCB41Pua7ZP8T2oFlGRttBKI7Du1vlF6WBBU/YHQqG9mv3giVo3rWsgIYOSbAVFUPvTgnrbmaSJIdQqzL6vr7bR3KIXBJUQ1EZeHHaB9TK2gCAzxZP9XErZiFk08fJwZ1w5QfEnivh7joog17HbINnZeuDsmdq4eP5tMOoZX4oI9iy26q/aJf5vzWfkX/EFWwYkk6u4073FWBeFRrIclUaFERRI3eTXmZnFwGjT47h5YeFBXFWqH5nUkLgpGknIlX7jlNIvspGB00E5UoAFIXscXqt/Aisdl/8j5YGg7tOWkOFmgznHqk9b+hTZSZvUPSXFxmIwFB2VuSeOYOU2zwk1ZGVSAtr2ohTu6GabeGcGCfRoOiWdlvmtqQwjeKbTPETYbgpmSrclAOYiG/oawUbD8Jd4o5+b4T1AhY6awJbbG26ZMWt1orYGZQJOe1Sk8NMa5S0Mpg6yOPnd8qs83QHDjPOc9K+ng6+513SOWY3YwOjFLty5GEPloUjuMOomNWLJD7adtUJGvTgo+p+yAcArcOzamBML+3l7OSeK28/bjP9Yh+sN9SxwSsSlI5AKyaTL+5jeURGeBFlDRHzKLY4qc2mntQpHut5w07o+UpNEDUlg8R0xYM0DdE3KzN7EbiUZU3XwF+4WnGCa2sQQlrm52FixqOnZipsJLkaBvDrOwEffgw1mpwWnFepE/gCPlgKWuR6CK36Zh0L+R+pPl6vVgs/vz5M99ipPHx8RFSK8lCx/l+JA8qPpCkDaW8OqnGEfAiGR9T1c65DJPGDSB674EeAVv+BfqEfTYKwpx0zsWZ4z5OQymxpIeu523ZuhchCZ30zkc88I47UpOdifMeSHKt2zAStDbW3uyzViYDyUOvgFBPo+S1mKmK11EWc0QH8ndOHhI68H6CadP4AqtdIGWuEd2wCtdXOBB2eMmlXg9sechOk70J+wXCWcNXeK3SVH826LLu9K5GKX2PiY9DuFlA0SEvguxUcOsP1reXVMDS5HCULBWS4vZRgH33JMMNZ2gK3fMdt3fBqd/VMKwR1GjoSo1B2zASCCWeV1kNkFUkGyF3eHEOgvyNWSqp7ZBP8K+39gWuLQmFDlET+5AAP0k7XW0dkfpX4iCqwKZeoqNswxCIWz9Vb0X6j3I899x7Px3k9mXSpp90juUTe4F5hljzYeyLIa3dO9FFLqQZDPbRkffGOQDkNY149gSTLkWraBNeAvFwVsD315vTPx/7zory9rkVyLkYmJQmibgsNIQ9yzOsBunWyYTTX8L3Eq4V56SxBhgNAsMTmgbIYDcPPxM+Jj/9AsjvqzujlSEXaZpgKQ2txhD0vgh09kgWhx3m/4xJXRRMHfZxQmucXEUsD/uhfv0pzO/SYM2XWkSb/mBlH/cEApPljWlMkBPmpKVAn02FVYvIzv6xWBByj/I+PrA25qAyHmtM/FdaepFqmAYc2+9Sx4G4IHoDu9nKADi31sYW0z5YryZTiMqpcD8ZEcVhHmOREFbs9VG8H1/ORdrpzsilTFp6kf5CDaJAPI9eDgMmjEkPHwNgb6JpTdCs3Z1kcdeTGKTpPQ0kz+hKiXzi5qDLQihu9J1Epj/Bw8W4liYa5qB+75ohzT/4QaM+IQ8bkadi2dCXRHJrTVtusd6GxshEmkgAkVtctDtSuFbdwThcEt8fD+7oXX66vQ65aJFELlmTRU3Q7BRLYQQnqWpbU8dBdA0REU6NO+9YA6zm9czUA7POaGXI5Ofia+q4f5Dyc/2z/rB783JzcrUsuctPM/MZeYiVrgfSZFErgi2rYZLSIXbeO0mjOBZ1aFjkS4pB4u5vlWgcokqR0clxd5OyPHTSlSz5ZejyKK27kMto81hTK2inTEubLE7b5HKE79TS5Sfvxqp0f3JS1JdrF10HmI8ZJvnV8npiZBpKk5jf7xICR81XaqCnRQ45W9hOYU0W9VAfbdPbIgU34K45O1EA2G1accl1XWA+hq8zLsKgN0MldiE90nqyNN8Q9r0yRhKgI3Gje0iA+HKupOlXu7s749VgGQzRpBJLiPZFx87wqq2EZnW2qrgEi38gx3f3YUxNLC3rN0vVIUgK5LE3kRAgDsfIobYtGlyNnEVU1TYtccl8STeGhEtokLQcuKrPzAvKyFYy4HknX0ZatpWT96xF6VByOy7xTxM7hYSVtT+sTsNL+M5FOEaJ9psR/jh8GqIBQ8B8zMwLim9JkTTpilw0lJgDJEvVLrdcmt8qlXacxHEjUi/r46+ISxfayantWd5Kl1dO2m7WgiEeq5KugSXAuRxGXtABCbBSAxY3wU09VsRt/15uBzW+lWfXX4fEjXBOGunXEdsWbVJ+w3c6U+uak4HKSyrKe77Udi6T3FrURrWIeqlc0RJC32MqhnF6XCVJBs0ua3Ou0guQCAHifFccjul4QfS0ZTWMXJZ1v7ELS0s1RVV1g/P+ImI+1g+qf8pSN7j5ipuZJkWBRNuo7mrRyHh1dv1niWuONGHENawiTs1uWQ1jX5fYG3bx7gZ6s1r9IDeu6pO96l8Sm9HGIfsIU9gmJGk1h9tzdgyuFlnU5gjS2V2Dbs0wLyemM251Ysf3RLe7lKkjuvz3Yj/qRRPBaneMw3yM5F/kQBrxljiBWaFPHGkijs2lgayrSwjCvcsoHSxuFKBXkbBynE7z2e5SpvBGKfrI22e0tLdY7aRYXDcHisj2poA9XuVFZdi4jiNNODVMGlWljJZ1lEX7PrekJNqN21mSfp9x6QDr+/0PAPZJoWWPXFnHwGW0LswTz4GkgJQb+5iHaKXUx8KOt0rOIbg39SNIcX6dZzHkGsYutFNwi4Dk0vJ2V7yXwYXr8EYTMOq13//EXxVn2pWA6GYVu4YbmmvtlrSeNC3a80/Nbv8Q6rmgcJBmMOSKd+Izia94r+jk0RzqCO4r1rxD0Fw+iDmWyZWXQJK7Zqs8WVgS69Qn0q7MxHLR2Dz2q4SDVP37TXFBSdzIxgSIuZatYzutk3IYhCTGOE3/MFHxMsPgA/q96ndrctN5hSML6zXa4wC7K9XLtxu9CocqarJju/cvwJ6CDTy2JxzyRP8L/vB1yfe1B79WIWBNH6WqcXff+MxBOTFuVdLr7FGh39lVWdPTL/BnkbWLp+KgOnCOYLVUzp7xIKVQSsmjn5CmTl04KZwUOTiHWUSxWrTowaet0ed7eg93YgvvtXV/lH81BoubS9F3HRVW3my333P79uPZy7z1DRUH/NswnQSj1fH1ydHR9fFqMQoms//vo3HAAQcccMABBxxwwAEHHHDAAQ3wX7Qrn6hJf12FAAAAAElFTkSuQmCC</t>
+  </si>
+  <si>
+    <t>https://cdn-images-1.medium.com/max/1200/1*Dw4-tOJ_9myFUywLd3qzjA.png</t>
+  </si>
+  <si>
+    <t>https://thearea.org/wp-content/uploads/2019/03/qc_logo_dml_rgb_blu_pos.png</t>
+  </si>
+  <si>
+    <t>https://g.foolcdn.com/art/companylogos/medium/REGN.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/en/thumb/f/f7/Ross_Stores_logo.svg/1200px-Ross_Stores_logo.svg.png</t>
+  </si>
+  <si>
+    <t>https://i.pcmag.com/imagery/reviews/02NI5TtZ2SlHLoJdMkRtvwi-7..v_1582315481.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/en/thumb/5/51/Skyworks_logo.svg/1200px-Skyworks_logo.svg.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/en/thumb/d/d3/Starbucks_Corporation_Logo_2011.svg/1200px-Starbucks_Corporation_Logo_2011.svg.png</t>
+  </si>
+  <si>
+    <t>https://www.synopsys.com/content/dam/synopsys/company/about/legal/synopsys-logos/colorlogo/synopsys_color.jpg</t>
+  </si>
+  <si>
+    <t>https://download.logo.wine/logo/Take-Two_Interactive/Take-Two_Interactive-Logo.wine.png</t>
+  </si>
+  <si>
+    <t>https://www.carlogos.org/car-logos/tesla-logo-2200x2800.png</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/content/dam/ticom/images/identities/ti-brand/ti-stk-2c-pos-rgb-logo.png</t>
+  </si>
+  <si>
+    <t>https://cached.imagescaler.hbpl.co.uk/resize/scaleHeight/815/cached.offlinehbpl.hbpl.co.uk/news/SUC/kraftheinz-20200320023814159.png</t>
+  </si>
+  <si>
+    <t>https://www.smartcellular.co.uk/pub/media/catalog/product/cache/39c1497ea30628584f6df05bad91eace/t/-/t-mobile.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/en/thumb/9/9e/Ulta_Beauty_logo.svg/1280px-Ulta_Beauty_logo.svg.png</t>
+  </si>
+  <si>
+    <t>https://digital.hbs.edu/platform-rctom/wp-content/uploads/sites/4/2015/12/Logo_Verisk_Analytics.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/en/thumb/d/d9/Vertex_logo.svg/1200px-Vertex_logo.svg.png</t>
+  </si>
+  <si>
+    <t>https://d53bpfpeyyyn7.cloudfront.net/Pictures/2000x2000fit/9/4/0/3076940_walgreensbootslogo_457232_crop.png</t>
+  </si>
+  <si>
+    <t>https://lh3.googleusercontent.com/proxy/UKY-iNfS23KCyMKXO4KQN0RMNni_zkTWGapy5OMeAK5Fw8peVMgz-y-Hx1pIGLHWtW-yeGmOENOjfuGgQY1443MW_j5AeAmMHThyGMw</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/3/3b/Workday_Logo.png</t>
   </si>
 </sst>
 </file>
@@ -859,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:BK83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -931,190 +1117,190 @@
   <sheetData>
     <row r="2" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" t="s">
         <v>75</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>76</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>77</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>78</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>79</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>80</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>81</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>82</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>83</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>84</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>85</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>86</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>87</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>88</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>89</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>90</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>91</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>92</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>93</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>94</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>95</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>96</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>97</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>98</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>99</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>100</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>101</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>102</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>103</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>104</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>105</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>106</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>107</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
         <v>108</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>109</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AN2" t="s">
         <v>110</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>111</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>112</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
         <v>113</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AR2" t="s">
         <v>114</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
         <v>115</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AT2" t="s">
         <v>116</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AU2" t="s">
         <v>117</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="AV2" t="s">
         <v>118</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="AW2" t="s">
         <v>119</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="AX2" t="s">
         <v>120</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="AY2" t="s">
         <v>121</v>
       </c>
-      <c r="AY2" t="s">
+      <c r="AZ2" t="s">
         <v>122</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="BA2" t="s">
         <v>123</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BB2" t="s">
         <v>124</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BC2" t="s">
         <v>125</v>
       </c>
-      <c r="BC2" t="s">
+      <c r="BD2" t="s">
         <v>126</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BE2" t="s">
         <v>127</v>
       </c>
-      <c r="BE2" t="s">
+      <c r="BF2" t="s">
         <v>128</v>
       </c>
-      <c r="BF2" t="s">
+      <c r="BG2" t="s">
         <v>129</v>
       </c>
-      <c r="BG2" t="s">
+      <c r="BH2" t="s">
         <v>130</v>
       </c>
-      <c r="BH2" t="s">
+      <c r="BI2" t="s">
         <v>131</v>
       </c>
-      <c r="BI2" t="s">
+      <c r="BJ2" t="s">
         <v>132</v>
       </c>
-      <c r="BJ2" t="s">
+      <c r="BK2" t="s">
         <v>133</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="3" spans="2:63" x14ac:dyDescent="0.2">
@@ -1122,7 +1308,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D3">
         <v>20.239999999999998</v>
@@ -1310,7 +1496,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D4">
         <v>72.699996999999996</v>
@@ -1498,7 +1684,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D5">
         <v>186.63999899999999</v>
@@ -1686,7 +1872,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D6">
         <v>57.240001999999997</v>
@@ -1871,10 +2057,10 @@
     </row>
     <row r="7" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D7">
         <v>527.56158400000004</v>
@@ -2067,7 +2253,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D9">
         <v>312.57998700000002</v>
@@ -2255,7 +2441,7 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D10">
         <v>2.67</v>
@@ -2443,7 +2629,7 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D11">
         <v>160.16000399999999</v>
@@ -2631,7 +2817,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D12">
         <v>55.68</v>
@@ -2819,7 +3005,7 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D13">
         <v>111.389999</v>
@@ -3007,7 +3193,7 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D14">
         <v>24.99</v>
@@ -3195,7 +3381,7 @@
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D15">
         <v>107.66999800000001</v>
@@ -3383,7 +3569,7 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D16">
         <v>60.060001</v>
@@ -3571,7 +3757,7 @@
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D17">
         <v>82.980002999999996</v>
@@ -3759,7 +3945,7 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D18">
         <v>229.46000699999999</v>
@@ -3947,7 +4133,7 @@
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D19">
         <v>342.83999599999999</v>
@@ -4135,7 +4321,7 @@
         <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D20">
         <v>91.239998</v>
@@ -4323,7 +4509,7 @@
         <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D21">
         <v>100.93</v>
@@ -4510,6 +4696,9 @@
       <c r="B22" t="s">
         <v>18</v>
       </c>
+      <c r="C22" t="s">
+        <v>160</v>
+      </c>
       <c r="D22">
         <v>19.149999999999999</v>
       </c>
@@ -4695,6 +4884,9 @@
       <c r="B23" t="s">
         <v>19</v>
       </c>
+      <c r="C23" t="s">
+        <v>161</v>
+      </c>
       <c r="D23">
         <v>64.919998000000007</v>
       </c>
@@ -4878,7 +5070,10 @@
     </row>
     <row r="24" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>136</v>
+        <v>135</v>
+      </c>
+      <c r="C24" t="s">
+        <v>162</v>
       </c>
       <c r="D24">
         <v>167.229996</v>
@@ -5065,6 +5260,9 @@
       <c r="B25" t="s">
         <v>20</v>
       </c>
+      <c r="C25" t="s">
+        <v>163</v>
+      </c>
       <c r="D25">
         <v>78.779999000000004</v>
       </c>
@@ -5250,6 +5448,9 @@
       <c r="B26" t="s">
         <v>21</v>
       </c>
+      <c r="C26" t="s">
+        <v>164</v>
+      </c>
       <c r="D26">
         <v>78.910004000000001</v>
       </c>
@@ -5435,6 +5636,9 @@
       <c r="B27" t="s">
         <v>22</v>
       </c>
+      <c r="C27" t="s">
+        <v>165</v>
+      </c>
       <c r="D27">
         <v>27.860001</v>
       </c>
@@ -5620,6 +5824,9 @@
       <c r="B28" t="s">
         <v>23</v>
       </c>
+      <c r="C28" t="s">
+        <v>166</v>
+      </c>
       <c r="D28">
         <v>50.907786999999999</v>
       </c>
@@ -5805,6 +6012,9 @@
       <c r="B29" t="s">
         <v>24</v>
       </c>
+      <c r="C29" t="s">
+        <v>167</v>
+      </c>
       <c r="D29">
         <v>52.889999000000003</v>
       </c>
@@ -5990,6 +6200,9 @@
       <c r="B30" t="s">
         <v>25</v>
       </c>
+      <c r="C30" t="s">
+        <v>168</v>
+      </c>
       <c r="D30">
         <v>29</v>
       </c>
@@ -6175,6 +6388,9 @@
       <c r="B31" t="s">
         <v>26</v>
       </c>
+      <c r="C31" t="s">
+        <v>169</v>
+      </c>
       <c r="D31">
         <v>141.86999499999999</v>
       </c>
@@ -6360,6 +6576,9 @@
       <c r="B32" t="s">
         <v>27</v>
       </c>
+      <c r="C32" t="s">
+        <v>170</v>
+      </c>
       <c r="D32">
         <v>36.110000999999997</v>
       </c>
@@ -6545,6 +6764,9 @@
       <c r="B33" t="s">
         <v>28</v>
       </c>
+      <c r="C33" t="s">
+        <v>171</v>
+      </c>
       <c r="D33">
         <v>70.940002000000007</v>
       </c>
@@ -6730,6 +6952,9 @@
       <c r="B34" t="s">
         <v>29</v>
       </c>
+      <c r="C34" t="s">
+        <v>172</v>
+      </c>
       <c r="D34">
         <v>23.728956</v>
       </c>
@@ -6915,6 +7140,9 @@
       <c r="B35" t="s">
         <v>30</v>
       </c>
+      <c r="C35" t="s">
+        <v>173</v>
+      </c>
       <c r="D35">
         <v>47.189999</v>
       </c>
@@ -7100,6 +7328,9 @@
       <c r="B36" t="s">
         <v>31</v>
       </c>
+      <c r="C36" t="s">
+        <v>174</v>
+      </c>
       <c r="D36">
         <v>85.580001999999993</v>
       </c>
@@ -7285,6 +7516,9 @@
       <c r="B37" t="s">
         <v>32</v>
       </c>
+      <c r="C37" t="s">
+        <v>175</v>
+      </c>
       <c r="D37">
         <v>78.580001999999993</v>
       </c>
@@ -7470,6 +7704,9 @@
       <c r="B38" t="s">
         <v>33</v>
       </c>
+      <c r="C38" t="s">
+        <v>176</v>
+      </c>
       <c r="D38">
         <v>23.924999</v>
       </c>
@@ -7655,6 +7892,9 @@
       <c r="B39" t="s">
         <v>34</v>
       </c>
+      <c r="C39" t="s">
+        <v>177</v>
+      </c>
       <c r="D39">
         <v>35.744999</v>
       </c>
@@ -7840,6 +8080,9 @@
       <c r="B40" t="s">
         <v>35</v>
       </c>
+      <c r="C40" t="s">
+        <v>178</v>
+      </c>
       <c r="D40">
         <v>95.139999000000003</v>
       </c>
@@ -8025,6 +8268,9 @@
       <c r="B41" t="s">
         <v>36</v>
       </c>
+      <c r="C41" t="s">
+        <v>179</v>
+      </c>
       <c r="D41">
         <v>74.315002000000007</v>
       </c>
@@ -8210,6 +8456,9 @@
       <c r="B42" t="s">
         <v>37</v>
       </c>
+      <c r="C42" t="s">
+        <v>180</v>
+      </c>
       <c r="D42">
         <v>186.16999799999999</v>
       </c>
@@ -8395,6 +8644,9 @@
       <c r="B43" t="s">
         <v>38</v>
       </c>
+      <c r="C43" t="s">
+        <v>181</v>
+      </c>
       <c r="D43">
         <v>73.650002000000001</v>
       </c>
@@ -8580,6 +8832,9 @@
       <c r="B44" t="s">
         <v>39</v>
       </c>
+      <c r="C44" t="s">
+        <v>182</v>
+      </c>
       <c r="D44">
         <v>36.669998</v>
       </c>
@@ -8765,6 +9020,9 @@
       <c r="B45" t="s">
         <v>40</v>
       </c>
+      <c r="C45" t="s">
+        <v>183</v>
+      </c>
       <c r="D45">
         <v>92.209998999999996</v>
       </c>
@@ -8950,6 +9208,9 @@
       <c r="B46" t="s">
         <v>41</v>
       </c>
+      <c r="C46" t="s">
+        <v>184</v>
+      </c>
       <c r="D46">
         <v>176.96000699999999</v>
       </c>
@@ -9135,6 +9396,9 @@
       <c r="B47" t="s">
         <v>42</v>
       </c>
+      <c r="C47" t="s">
+        <v>185</v>
+      </c>
       <c r="D47">
         <v>23.370000999999998</v>
       </c>
@@ -9320,6 +9584,9 @@
       <c r="B48" t="s">
         <v>43</v>
       </c>
+      <c r="C48" t="s">
+        <v>186</v>
+      </c>
       <c r="D48">
         <v>70.620002999999997</v>
       </c>
@@ -9505,6 +9772,9 @@
       <c r="B49" t="s">
         <v>44</v>
       </c>
+      <c r="C49" t="s">
+        <v>187</v>
+      </c>
       <c r="D49">
         <v>79.870002999999997</v>
       </c>
@@ -9690,6 +9960,9 @@
       <c r="B50" t="s">
         <v>45</v>
       </c>
+      <c r="C50" t="s">
+        <v>188</v>
+      </c>
       <c r="D50">
         <v>50.490001999999997</v>
       </c>
@@ -9875,6 +10148,9 @@
       <c r="B51" t="s">
         <v>46</v>
       </c>
+      <c r="C51" t="s">
+        <v>189</v>
+      </c>
       <c r="D51">
         <v>78.339995999999999</v>
       </c>
@@ -10060,6 +10336,9 @@
       <c r="B52" t="s">
         <v>47</v>
       </c>
+      <c r="C52" t="s">
+        <v>190</v>
+      </c>
       <c r="D52">
         <v>31.98</v>
       </c>
@@ -10245,6 +10524,9 @@
       <c r="B53" t="s">
         <v>48</v>
       </c>
+      <c r="C53" t="s">
+        <v>191</v>
+      </c>
       <c r="D53">
         <v>127.900002</v>
       </c>
@@ -10430,6 +10712,9 @@
       <c r="B54" t="s">
         <v>49</v>
       </c>
+      <c r="C54" t="s">
+        <v>192</v>
+      </c>
       <c r="D54">
         <v>45.360000999999997</v>
       </c>
@@ -10615,6 +10900,9 @@
       <c r="B55" t="s">
         <v>50</v>
       </c>
+      <c r="C55" t="s">
+        <v>193</v>
+      </c>
       <c r="D55">
         <v>35.240001999999997</v>
       </c>
@@ -10800,6 +11088,9 @@
       <c r="B56" t="s">
         <v>51</v>
       </c>
+      <c r="C56" t="s">
+        <v>194</v>
+      </c>
       <c r="D56">
         <v>46.66</v>
       </c>
@@ -10985,6 +11276,9 @@
       <c r="B57" t="s">
         <v>52</v>
       </c>
+      <c r="C57" t="s">
+        <v>195</v>
+      </c>
       <c r="D57">
         <v>36.43</v>
       </c>
@@ -11168,7 +11462,10 @@
     </row>
     <row r="58" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>53</v>
+        <v>197</v>
+      </c>
+      <c r="C58" t="s">
+        <v>196</v>
       </c>
       <c r="D58">
         <v>36.466667000000001</v>
@@ -11353,7 +11650,10 @@
     </row>
     <row r="59" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="C59" t="s">
+        <v>198</v>
       </c>
       <c r="D59">
         <v>99.82</v>
@@ -11538,7 +11838,10 @@
     </row>
     <row r="60" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="C60" t="s">
+        <v>199</v>
       </c>
       <c r="D60">
         <v>49.151428000000003</v>
@@ -11723,7 +12026,10 @@
     </row>
     <row r="61" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="C61" t="s">
+        <v>200</v>
       </c>
       <c r="D61">
         <v>20.129999000000002</v>
@@ -11908,7 +12214,10 @@
     </row>
     <row r="62" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>137</v>
+        <v>136</v>
+      </c>
+      <c r="C62" t="s">
+        <v>201</v>
       </c>
       <c r="D62">
         <v>192.86000100000001</v>
@@ -12093,7 +12402,10 @@
     </row>
     <row r="63" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="C63" t="s">
+        <v>202</v>
       </c>
       <c r="D63">
         <v>68.220000999999996</v>
@@ -12278,7 +12590,10 @@
     </row>
     <row r="64" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="C64" t="s">
+        <v>203</v>
       </c>
       <c r="D64">
         <v>46.360000999999997</v>
@@ -12463,7 +12778,10 @@
     </row>
     <row r="65" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="C65" t="s">
+        <v>204</v>
       </c>
       <c r="D65">
         <v>38</v>
@@ -12630,7 +12948,10 @@
     </row>
     <row r="66" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="C66" t="s">
+        <v>205</v>
       </c>
       <c r="D66">
         <v>74.510002</v>
@@ -12815,7 +13136,10 @@
     </row>
     <row r="67" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="C67" t="s">
+        <v>206</v>
       </c>
       <c r="D67">
         <v>413.89999399999999</v>
@@ -13000,7 +13324,10 @@
     </row>
     <row r="68" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="C68" t="s">
+        <v>207</v>
       </c>
       <c r="D68">
         <v>47.419998</v>
@@ -13185,7 +13512,10 @@
     </row>
     <row r="69" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="C69" t="s">
+        <v>208</v>
       </c>
       <c r="D69">
         <v>3.5</v>
@@ -13370,7 +13700,10 @@
     </row>
     <row r="70" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="C70" t="s">
+        <v>209</v>
       </c>
       <c r="D70">
         <v>73.599997999999999</v>
@@ -13555,7 +13888,10 @@
     </row>
     <row r="71" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="C71" t="s">
+        <v>210</v>
       </c>
       <c r="D71">
         <v>41.064999</v>
@@ -13740,7 +14076,10 @@
     </row>
     <row r="72" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="C72" t="s">
+        <v>211</v>
       </c>
       <c r="D72">
         <v>43.73</v>
@@ -13925,7 +14264,10 @@
     </row>
     <row r="73" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="C73" t="s">
+        <v>212</v>
       </c>
       <c r="D73">
         <v>28.200001</v>
@@ -14110,7 +14452,10 @@
     </row>
     <row r="74" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="C74" t="s">
+        <v>213</v>
       </c>
       <c r="D74">
         <v>222.86999499999999</v>
@@ -14295,7 +14640,10 @@
     </row>
     <row r="75" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+      <c r="C75" t="s">
+        <v>214</v>
       </c>
       <c r="D75">
         <v>53.560001</v>
@@ -14480,7 +14828,10 @@
     </row>
     <row r="76" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="C76" t="s">
+        <v>215</v>
       </c>
       <c r="D76">
         <v>80</v>
@@ -14644,7 +14995,10 @@
     </row>
     <row r="77" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
-        <v>138</v>
+        <v>137</v>
+      </c>
+      <c r="C77" t="s">
+        <v>216</v>
       </c>
       <c r="D77">
         <v>27.1</v>
@@ -14829,7 +15183,10 @@
     </row>
     <row r="78" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="C78" t="s">
+        <v>217</v>
       </c>
       <c r="D78">
         <v>128.13000500000001</v>
@@ -15014,7 +15371,10 @@
     </row>
     <row r="79" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
-        <v>139</v>
+        <v>138</v>
+      </c>
+      <c r="C79" t="s">
+        <v>218</v>
       </c>
       <c r="D79">
         <v>64.080001999999993</v>
@@ -15199,7 +15559,10 @@
     </row>
     <row r="80" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="C80" t="s">
+        <v>219</v>
       </c>
       <c r="D80">
         <v>119.970001</v>
@@ -15384,7 +15747,10 @@
     </row>
     <row r="81" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="C81" t="s">
+        <v>220</v>
       </c>
       <c r="D81">
         <v>76.110000999999997</v>
@@ -15569,7 +15935,10 @@
     </row>
     <row r="82" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="C82" t="s">
+        <v>221</v>
       </c>
       <c r="D82">
         <v>111.800003</v>
@@ -15754,7 +16123,10 @@
     </row>
     <row r="83" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
-        <v>140</v>
+        <v>139</v>
+      </c>
+      <c r="C83" t="s">
+        <v>222</v>
       </c>
       <c r="D83">
         <v>81.819999999999993</v>

</xml_diff>